<commit_message>
updated charts time of day
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neal\Desktop\GroupC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B77B461-86E4-4389-B747-FBAC3DA70E82}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68043E7E-205E-4F74-B74E-5E66703FEA9E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9B31D286-B249-4856-AC8C-42ACBBB5A474}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="179021"/>
   <extLst>
@@ -1533,6 +1534,377 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Crimes by Time of Day </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[4]Sheet7!$K$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6011-459C-A56E-3A244A593B03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6011-459C-A56E-3A244A593B03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[4]Sheet7!$J$9:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Day (6AM-6PM)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Night (6PM-6AM)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[4]Sheet7!$K$9:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.34488170667906759</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65511829332093241</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6011-459C-A56E-3A244A593B03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5247,6 +5619,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7567,6 +7979,525 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="262">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -12168,6 +13099,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B8E3005-5BA4-42B5-8A8D-C57103E94458}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12930,6 +13899,55 @@
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="Sheet4"/>
+      <sheetName val="Sheet5"/>
+      <sheetName val="Sheet7"/>
+      <sheetName val="Sheet8"/>
+      <sheetName val="Sheet9"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
+        <row r="8">
+          <cell r="K8" t="str">
+            <v>%</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="J9" t="str">
+            <v>Day (6AM-6PM)</v>
+          </cell>
+          <cell r="K9">
+            <v>0.34488170667906759</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="J10" t="str">
+            <v>Night (6PM-6AM)</v>
+          </cell>
+          <cell r="K10">
+            <v>0.65511829332093241</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -13234,8 +14252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A741AFA-65C7-47ED-807E-17D5FD606870}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="R84" sqref="R84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update to charts, PowerPoint
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neal\Desktop\GroupC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68043E7E-205E-4F74-B74E-5E66703FEA9E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11866AE5-66E1-4476-84B5-6F87728D9298}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9B31D286-B249-4856-AC8C-42ACBBB5A474}"/>
   </bookViews>
@@ -1796,10 +1796,10 @@
             </c:txPr>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
+            <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
@@ -14252,8 +14252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A741AFA-65C7-47ED-807E-17D5FD606870}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="R84" sqref="R84"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>